<commit_message>
Added z_level parameter to pyecharts objects
</commit_message>
<xml_diff>
--- a/vbp.xlsx
+++ b/vbp.xlsx
@@ -2807,8 +2807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="M76" sqref="M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2927,8 +2927,8 @@
       <c r="I4" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J4" s="35">
-        <v>6.6</v>
+      <c r="J4" s="39">
+        <v>0.94285714285714284</v>
       </c>
       <c r="K4" s="35"/>
       <c r="L4" s="36">
@@ -2966,8 +2966,8 @@
       <c r="I5" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J5" s="35">
-        <v>6.6</v>
+      <c r="J5" s="39">
+        <v>0.94285714285714284</v>
       </c>
       <c r="K5" s="35"/>
       <c r="L5" s="36">
@@ -3005,8 +3005,8 @@
       <c r="I6" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J6" s="35">
-        <v>6.6</v>
+      <c r="J6" s="39">
+        <v>0.94285714285714284</v>
       </c>
       <c r="K6" s="38">
         <v>2.6084012278529012</v>
@@ -3046,8 +3046,8 @@
       <c r="I7" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J7" s="35">
-        <v>6.6</v>
+      <c r="J7" s="39">
+        <v>0.94285714285714284</v>
       </c>
       <c r="K7" s="38">
         <v>3.5186050989002973</v>
@@ -3085,8 +3085,8 @@
       <c r="I8" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J8" s="35">
-        <v>6.6</v>
+      <c r="J8" s="39">
+        <v>0.94285714285714284</v>
       </c>
       <c r="K8" s="38">
         <v>6.4316864721008642</v>
@@ -3124,8 +3124,8 @@
       <c r="I9" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J9" s="35">
-        <v>21.8</v>
+      <c r="J9" s="39">
+        <v>0.77857142857142858</v>
       </c>
       <c r="K9" s="39">
         <v>2.5164968727809582</v>
@@ -3165,8 +3165,8 @@
       <c r="I10" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J10" s="35">
-        <v>21.8</v>
+      <c r="J10" s="39">
+        <v>0.77857142857142858</v>
       </c>
       <c r="K10" s="39"/>
       <c r="L10" s="36">
@@ -3204,8 +3204,8 @@
       <c r="I11" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J11" s="35">
-        <v>21.8</v>
+      <c r="J11" s="39">
+        <v>0.77857142857142858</v>
       </c>
       <c r="K11" s="39">
         <v>2.8987411715941023</v>
@@ -3245,8 +3245,8 @@
       <c r="I12" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J12" s="35">
-        <v>21.8</v>
+      <c r="J12" s="39">
+        <v>0.77857142857142858</v>
       </c>
       <c r="K12" s="39">
         <v>3.1717676127624475</v>
@@ -3284,8 +3284,8 @@
       <c r="I13" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="35">
-        <v>21.8</v>
+      <c r="J13" s="39">
+        <v>0.77857142857142858</v>
       </c>
       <c r="K13" s="39">
         <v>4.0205626355092319</v>
@@ -3323,8 +3323,8 @@
       <c r="I14" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J14" s="35">
-        <v>21.8</v>
+      <c r="J14" s="39">
+        <v>0.77857142857142858</v>
       </c>
       <c r="K14" s="39">
         <v>6.311494245862975</v>
@@ -3362,8 +3362,8 @@
       <c r="I15" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J15" s="35">
-        <v>22.26</v>
+      <c r="J15" s="39">
+        <v>3.18</v>
       </c>
       <c r="K15" s="39"/>
       <c r="L15" s="36">
@@ -3401,8 +3401,8 @@
       <c r="I16" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J16" s="35">
-        <v>22.26</v>
+      <c r="J16" s="39">
+        <v>3.18</v>
       </c>
       <c r="K16" s="39">
         <v>15.924687470932279</v>
@@ -3442,8 +3442,8 @@
       <c r="I17" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J17" s="35">
-        <v>22.26</v>
+      <c r="J17" s="39">
+        <v>3.18</v>
       </c>
       <c r="K17" s="39">
         <v>6.7403919498047147</v>
@@ -3483,8 +3483,8 @@
       <c r="I18" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J18" s="35">
-        <v>22.26</v>
+      <c r="J18" s="39">
+        <v>3.18</v>
       </c>
       <c r="K18" s="39">
         <v>8.2071950252433599</v>
@@ -3522,8 +3522,8 @@
       <c r="I19" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J19" s="35">
-        <v>5.66</v>
+      <c r="J19" s="39">
+        <v>0.20214285714285715</v>
       </c>
       <c r="K19" s="35"/>
       <c r="L19" s="36">
@@ -3561,8 +3561,8 @@
       <c r="I20" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J20" s="35">
-        <v>5.66</v>
+      <c r="J20" s="39">
+        <v>0.20214285714285715</v>
       </c>
       <c r="K20" s="39">
         <v>0.53531977685952137</v>
@@ -3602,8 +3602,8 @@
       <c r="I21" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J21" s="35">
-        <v>5.66</v>
+      <c r="J21" s="39">
+        <v>0.20214285714285715</v>
       </c>
       <c r="K21" s="39">
         <v>1.2931271822905741</v>
@@ -3643,8 +3643,8 @@
       <c r="I22" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J22" s="35">
-        <v>5.66</v>
+      <c r="J22" s="39">
+        <v>0.20214285714285715</v>
       </c>
       <c r="K22" s="39">
         <v>4.208464972161396</v>
@@ -3682,8 +3682,8 @@
       <c r="I23" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J23" s="35">
-        <v>4.16</v>
+      <c r="J23" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K23" s="39">
         <v>0.66231211342398322</v>
@@ -3723,8 +3723,8 @@
       <c r="I24" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J24" s="35">
-        <v>4.16</v>
+      <c r="J24" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K24" s="39">
         <v>0.59455887212248038</v>
@@ -3764,8 +3764,8 @@
       <c r="I25" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="35">
-        <v>4.16</v>
+      <c r="J25" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K25" s="39"/>
       <c r="L25" s="36">
@@ -3803,8 +3803,8 @@
       <c r="I26" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J26" s="35">
-        <v>4.16</v>
+      <c r="J26" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K26" s="39"/>
       <c r="L26" s="36">
@@ -3840,8 +3840,8 @@
       <c r="I27" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="35">
-        <v>4.16</v>
+      <c r="J27" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K27" s="39">
         <v>0.28382604300841285</v>
@@ -3879,8 +3879,8 @@
       <c r="I28" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J28" s="35">
-        <v>4.16</v>
+      <c r="J28" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K28" s="39">
         <v>0.7986175709404385</v>
@@ -3918,8 +3918,8 @@
       <c r="I29" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J29" s="35">
-        <v>4.16</v>
+      <c r="J29" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K29" s="35"/>
       <c r="L29" s="36">
@@ -3955,8 +3955,8 @@
       <c r="I30" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J30" s="35">
-        <v>4.16</v>
+      <c r="J30" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K30" s="39">
         <v>0.26541093880234318</v>
@@ -3994,8 +3994,8 @@
       <c r="I31" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J31" s="35">
-        <v>4.16</v>
+      <c r="J31" s="39">
+        <v>0.14857142857142858</v>
       </c>
       <c r="K31" s="35"/>
       <c r="L31" s="36">
@@ -4031,8 +4031,8 @@
       <c r="I32" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J32" s="35">
-        <v>17.36</v>
+      <c r="J32" s="39">
+        <v>0.62</v>
       </c>
       <c r="K32" s="39">
         <v>15.73692173407041</v>
@@ -4072,8 +4072,8 @@
       <c r="I33" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J33" s="35">
-        <v>17.36</v>
+      <c r="J33" s="39">
+        <v>0.62</v>
       </c>
       <c r="K33" s="39"/>
       <c r="L33" s="36">
@@ -4111,8 +4111,8 @@
       <c r="I34" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J34" s="35">
-        <v>17.36</v>
+      <c r="J34" s="39">
+        <v>0.62</v>
       </c>
       <c r="K34" s="39">
         <v>9.5726844583987436</v>
@@ -4152,8 +4152,8 @@
       <c r="I35" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J35" s="35">
-        <v>17.36</v>
+      <c r="J35" s="39">
+        <v>0.62</v>
       </c>
       <c r="K35" s="39">
         <v>10.459261501210653</v>
@@ -4191,8 +4191,8 @@
       <c r="I36" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J36" s="35">
-        <v>17.36</v>
+      <c r="J36" s="39">
+        <v>0.62</v>
       </c>
       <c r="K36" s="39">
         <v>6.6617964844549178</v>
@@ -4230,8 +4230,8 @@
       <c r="I37" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J37" s="35">
-        <v>17.36</v>
+      <c r="J37" s="39">
+        <v>0.62</v>
       </c>
       <c r="K37" s="39">
         <v>6.259532433775818</v>
@@ -4269,8 +4269,8 @@
       <c r="I38" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J38" s="35">
-        <v>17.36</v>
+      <c r="J38" s="39">
+        <v>0.62</v>
       </c>
       <c r="K38" s="39"/>
       <c r="L38" s="36">
@@ -4306,8 +4306,8 @@
       <c r="I39" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J39" s="35">
-        <v>17.36</v>
+      <c r="J39" s="39">
+        <v>0.62</v>
       </c>
       <c r="K39" s="39">
         <v>13.630900516340919</v>
@@ -4345,8 +4345,8 @@
       <c r="I40" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J40" s="35">
-        <v>17.36</v>
+      <c r="J40" s="39">
+        <v>0.62</v>
       </c>
       <c r="K40" s="39">
         <v>27.059155952321181</v>
@@ -4384,8 +4384,8 @@
       <c r="I41" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J41" s="35">
-        <v>30.94</v>
+      <c r="J41" s="39">
+        <v>4.42</v>
       </c>
       <c r="K41" s="35"/>
       <c r="L41" s="36">
@@ -4423,8 +4423,8 @@
       <c r="I42" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J42" s="35">
-        <v>30.94</v>
+      <c r="J42" s="39">
+        <v>4.42</v>
       </c>
       <c r="K42" s="39">
         <v>4.2712816910402962</v>
@@ -4464,8 +4464,8 @@
       <c r="I43" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J43" s="35">
-        <v>30.94</v>
+      <c r="J43" s="39">
+        <v>4.42</v>
       </c>
       <c r="K43" s="39">
         <v>6.8380250799343312</v>
@@ -4505,8 +4505,8 @@
       <c r="I44" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J44" s="35">
-        <v>30.94</v>
+      <c r="J44" s="39">
+        <v>4.42</v>
       </c>
       <c r="K44" s="35">
         <v>13.76</v>
@@ -4544,8 +4544,8 @@
       <c r="I45" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J45" s="35">
-        <v>33.4</v>
+      <c r="J45" s="39">
+        <v>1.67</v>
       </c>
       <c r="K45" s="35">
         <v>3.4</v>
@@ -4585,8 +4585,8 @@
       <c r="I46" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J46" s="35">
-        <v>33.4</v>
+      <c r="J46" s="39">
+        <v>1.67</v>
       </c>
       <c r="K46" s="35">
         <v>3.38</v>
@@ -4626,8 +4626,8 @@
       <c r="I47" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J47" s="35">
-        <v>33.4</v>
+      <c r="J47" s="39">
+        <v>1.67</v>
       </c>
       <c r="K47" s="35">
         <v>8.81</v>
@@ -4665,8 +4665,8 @@
       <c r="I48" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J48" s="35">
-        <v>67.510000000000005</v>
+      <c r="J48" s="39">
+        <v>9.644285714285715</v>
       </c>
       <c r="K48" s="35"/>
       <c r="L48" s="36">
@@ -4704,8 +4704,8 @@
       <c r="I49" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J49" s="35">
-        <v>67.510000000000005</v>
+      <c r="J49" s="39">
+        <v>9.644285714285715</v>
       </c>
       <c r="K49" s="35">
         <v>14.4</v>
@@ -4745,8 +4745,8 @@
       <c r="I50" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J50" s="35">
-        <v>67.510000000000005</v>
+      <c r="J50" s="39">
+        <v>9.644285714285715</v>
       </c>
       <c r="K50" s="35">
         <v>13.87</v>
@@ -4786,8 +4786,8 @@
       <c r="I51" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J51" s="35">
-        <v>67.510000000000005</v>
+      <c r="J51" s="39">
+        <v>9.644285714285715</v>
       </c>
       <c r="K51" s="35">
         <v>29.06</v>
@@ -4825,8 +4825,8 @@
       <c r="I52" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J52" s="35">
-        <v>6.16</v>
+      <c r="J52" s="39">
+        <v>0.51333333333333331</v>
       </c>
       <c r="K52" s="35">
         <v>2.54</v>
@@ -4866,8 +4866,8 @@
       <c r="I53" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J53" s="35">
-        <v>6.16</v>
+      <c r="J53" s="39">
+        <v>0.51333333333333331</v>
       </c>
       <c r="K53" s="35">
         <v>0.63</v>
@@ -4907,8 +4907,8 @@
       <c r="I54" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J54" s="35">
-        <v>6.16</v>
+      <c r="J54" s="39">
+        <v>0.51333333333333331</v>
       </c>
       <c r="K54" s="35">
         <v>0.64</v>
@@ -4948,8 +4948,8 @@
       <c r="I55" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J55" s="35">
-        <v>6.16</v>
+      <c r="J55" s="39">
+        <v>0.51333333333333331</v>
       </c>
       <c r="K55" s="35">
         <v>0.61</v>
@@ -4987,8 +4987,8 @@
       <c r="I56" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J56" s="35">
-        <v>6.16</v>
+      <c r="J56" s="39">
+        <v>0.51333333333333331</v>
       </c>
       <c r="K56" s="35"/>
       <c r="L56" s="36">
@@ -5024,8 +5024,8 @@
       <c r="I57" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J57" s="35">
-        <v>6.16</v>
+      <c r="J57" s="39">
+        <v>0.51333333333333331</v>
       </c>
       <c r="K57" s="35"/>
       <c r="L57" s="36">
@@ -5061,8 +5061,8 @@
       <c r="I58" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J58" s="35">
-        <v>6.16</v>
+      <c r="J58" s="39">
+        <v>0.51333333333333331</v>
       </c>
       <c r="K58" s="35">
         <v>2.85</v>
@@ -5100,8 +5100,8 @@
       <c r="I59" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J59" s="35">
-        <v>10.02</v>
+      <c r="J59" s="39">
+        <v>0.16699999999999998</v>
       </c>
       <c r="K59" s="35">
         <v>0.87</v>
@@ -5141,8 +5141,8 @@
       <c r="I60" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J60" s="35">
-        <v>10.02</v>
+      <c r="J60" s="39">
+        <v>0.16699999999999998</v>
       </c>
       <c r="K60" s="35">
         <v>1.28</v>
@@ -5182,8 +5182,8 @@
       <c r="I61" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J61" s="35">
-        <v>10.02</v>
+      <c r="J61" s="39">
+        <v>0.16699999999999998</v>
       </c>
       <c r="K61" s="35">
         <v>0.5</v>
@@ -5223,8 +5223,8 @@
       <c r="I62" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J62" s="35">
-        <v>10.02</v>
+      <c r="J62" s="39">
+        <v>0.16699999999999998</v>
       </c>
       <c r="K62" s="35">
         <v>1.08</v>
@@ -5262,8 +5262,8 @@
       <c r="I63" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J63" s="35">
-        <v>10.02</v>
+      <c r="J63" s="39">
+        <v>0.16699999999999998</v>
       </c>
       <c r="K63" s="35">
         <v>2.5499999999999998</v>
@@ -5301,8 +5301,8 @@
       <c r="I64" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J64" s="35">
-        <v>547</v>
+      <c r="J64" s="39">
+        <v>54.7</v>
       </c>
       <c r="K64" s="35">
         <v>162.15</v>
@@ -5342,8 +5342,8 @@
       <c r="I65" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="35">
-        <v>547</v>
+      <c r="J65" s="39">
+        <v>54.7</v>
       </c>
       <c r="K65" s="35"/>
       <c r="L65" s="36">
@@ -5381,8 +5381,8 @@
       <c r="I66" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J66" s="35">
-        <v>547</v>
+      <c r="J66" s="39">
+        <v>54.7</v>
       </c>
       <c r="K66" s="35">
         <v>236.22</v>
@@ -5422,8 +5422,8 @@
       <c r="I67" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J67" s="35">
-        <v>11.8</v>
+      <c r="J67" s="39">
+        <v>0.84285714285714286</v>
       </c>
       <c r="K67" s="35">
         <v>2.04</v>
@@ -5463,8 +5463,8 @@
       <c r="I68" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J68" s="35">
-        <v>11.8</v>
+      <c r="J68" s="39">
+        <v>0.84285714285714286</v>
       </c>
       <c r="K68" s="35">
         <v>2.84</v>
@@ -5504,8 +5504,8 @@
       <c r="I69" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J69" s="35">
-        <v>15.26</v>
+      <c r="J69" s="39">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K69" s="35">
         <v>2.5299999999999998</v>
@@ -5545,8 +5545,8 @@
       <c r="I70" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J70" s="35">
-        <v>15.26</v>
+      <c r="J70" s="39">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K70" s="35">
         <v>3.54</v>
@@ -5586,8 +5586,8 @@
       <c r="I71" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="35">
-        <v>15.26</v>
+      <c r="J71" s="39">
+        <v>1.0900000000000001</v>
       </c>
       <c r="K71" s="35">
         <v>4.3600000000000003</v>
@@ -5627,8 +5627,8 @@
       <c r="I72" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J72" s="35">
-        <v>6.45</v>
+      <c r="J72" s="39">
+        <v>0.23035714285714287</v>
       </c>
       <c r="K72" s="35">
         <v>1.19</v>
@@ -5668,8 +5668,8 @@
       <c r="I73" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J73" s="35">
-        <v>17.72</v>
+      <c r="J73" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K73" s="35"/>
       <c r="L73" s="36">
@@ -5707,8 +5707,8 @@
       <c r="I74" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J74" s="35">
-        <v>17.72</v>
+      <c r="J74" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K74" s="35"/>
       <c r="L74" s="36">
@@ -5746,8 +5746,8 @@
       <c r="I75" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J75" s="35">
-        <v>17.72</v>
+      <c r="J75" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K75" s="35">
         <v>13.34</v>
@@ -5787,8 +5787,8 @@
       <c r="I76" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J76" s="35">
-        <v>17.72</v>
+      <c r="J76" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K76" s="35"/>
       <c r="L76" s="36">
@@ -5824,8 +5824,8 @@
       <c r="I77" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J77" s="35">
-        <v>17.72</v>
+      <c r="J77" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K77" s="35"/>
       <c r="L77" s="36">
@@ -5861,8 +5861,8 @@
       <c r="I78" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J78" s="35">
-        <v>17.72</v>
+      <c r="J78" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K78" s="35">
         <v>14.19</v>
@@ -5900,8 +5900,8 @@
       <c r="I79" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J79" s="35">
-        <v>17.72</v>
+      <c r="J79" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K79" s="35"/>
       <c r="L79" s="36">
@@ -5937,8 +5937,8 @@
       <c r="I80" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J80" s="35">
-        <v>17.72</v>
+      <c r="J80" s="39">
+        <v>0.59066666666666667</v>
       </c>
       <c r="K80" s="35">
         <v>16.27</v>
@@ -5976,8 +5976,8 @@
       <c r="I81" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J81" s="35">
-        <v>14.7</v>
+      <c r="J81" s="39">
+        <v>1.05</v>
       </c>
       <c r="K81" s="35">
         <v>2.23</v>
@@ -6017,8 +6017,8 @@
       <c r="I82" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J82" s="35">
-        <v>8.93</v>
+      <c r="J82" s="39">
+        <v>0.55812499999999998</v>
       </c>
       <c r="K82" s="35">
         <v>1.07</v>
@@ -6058,8 +6058,8 @@
       <c r="I83" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J83" s="35">
-        <v>72</v>
+      <c r="J83" s="39">
+        <v>2.4</v>
       </c>
       <c r="K83" s="35">
         <v>3.18</v>
@@ -6099,8 +6099,8 @@
       <c r="I84" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J84" s="35">
-        <v>72</v>
+      <c r="J84" s="39">
+        <v>2.4</v>
       </c>
       <c r="K84" s="35"/>
       <c r="L84" s="36">
@@ -6138,8 +6138,8 @@
       <c r="I85" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J85" s="35">
-        <v>72</v>
+      <c r="J85" s="39">
+        <v>2.4</v>
       </c>
       <c r="K85" s="35">
         <v>4.55</v>
@@ -6177,8 +6177,8 @@
       <c r="I86" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J86" s="35">
-        <v>623.82000000000005</v>
+      <c r="J86" s="39">
+        <v>10.397</v>
       </c>
       <c r="K86" s="35">
         <v>15.04</v>
@@ -6218,8 +6218,8 @@
       <c r="I87" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J87" s="35">
-        <v>623.82000000000005</v>
+      <c r="J87" s="39">
+        <v>10.397</v>
       </c>
       <c r="K87" s="35">
         <v>18.91</v>
@@ -6259,8 +6259,8 @@
       <c r="I88" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="J88" s="35">
-        <v>623.82000000000005</v>
+      <c r="J88" s="39">
+        <v>10.397</v>
       </c>
       <c r="K88" s="35">
         <v>183.29</v>
@@ -6298,8 +6298,8 @@
       <c r="I89" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="J89" s="35">
-        <v>19.38</v>
+      <c r="J89" s="39">
+        <v>3.8759999999999999</v>
       </c>
       <c r="K89" s="35"/>
       <c r="L89" s="36">
@@ -6337,8 +6337,8 @@
       <c r="I90" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J90" s="35">
-        <v>19.38</v>
+      <c r="J90" s="39">
+        <v>3.8759999999999999</v>
       </c>
       <c r="K90" s="35">
         <v>6.92</v>
@@ -6378,8 +6378,8 @@
       <c r="I91" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J91" s="35">
-        <v>10.199999999999999</v>
+      <c r="J91" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K91" s="35">
         <v>1</v>
@@ -6419,8 +6419,8 @@
       <c r="I92" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J92" s="35">
-        <v>10.199999999999999</v>
+      <c r="J92" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K92" s="35">
         <v>1.76</v>
@@ -6460,8 +6460,8 @@
       <c r="I93" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J93" s="35">
-        <v>10.199999999999999</v>
+      <c r="J93" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K93" s="35">
         <v>0.68</v>
@@ -6501,8 +6501,8 @@
       <c r="I94" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J94" s="35">
-        <v>10.199999999999999</v>
+      <c r="J94" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K94" s="35">
         <v>0.85</v>
@@ -6540,8 +6540,8 @@
       <c r="I95" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J95" s="35">
-        <v>10.199999999999999</v>
+      <c r="J95" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K95" s="35">
         <v>0.78</v>
@@ -6579,8 +6579,8 @@
       <c r="I96" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J96" s="35">
-        <v>10.199999999999999</v>
+      <c r="J96" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K96" s="35">
         <v>0.66</v>
@@ -6618,8 +6618,8 @@
       <c r="I97" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J97" s="35">
-        <v>10.199999999999999</v>
+      <c r="J97" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K97" s="35">
         <v>0.4</v>
@@ -6657,8 +6657,8 @@
       <c r="I98" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J98" s="35">
-        <v>10.199999999999999</v>
+      <c r="J98" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K98" s="35">
         <v>0.52</v>
@@ -6696,8 +6696,8 @@
       <c r="I99" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J99" s="35">
-        <v>10.199999999999999</v>
+      <c r="J99" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K99" s="35">
         <v>0.81</v>
@@ -6735,8 +6735,8 @@
       <c r="I100" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J100" s="35">
-        <v>10.199999999999999</v>
+      <c r="J100" s="39">
+        <v>0.67999999999999994</v>
       </c>
       <c r="K100" s="35">
         <v>1.83</v>
@@ -6774,8 +6774,8 @@
       <c r="I101" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J101" s="35">
-        <v>2776.97</v>
+      <c r="J101" s="39">
+        <v>810</v>
       </c>
       <c r="K101" s="35"/>
       <c r="L101" s="36">
@@ -6813,8 +6813,8 @@
       <c r="I102" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J102" s="35">
-        <v>2776.97</v>
+      <c r="J102" s="39">
+        <v>810</v>
       </c>
       <c r="K102" s="35">
         <v>3322</v>
@@ -6854,8 +6854,8 @@
       <c r="I103" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J103" s="35">
-        <v>109.75</v>
+      <c r="J103" s="39">
+        <v>21.95</v>
       </c>
       <c r="K103" s="35">
         <v>63.7</v>
@@ -6895,8 +6895,8 @@
       <c r="I104" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J104" s="35">
-        <v>109.75</v>
+      <c r="J104" s="39">
+        <v>21.95</v>
       </c>
       <c r="K104" s="35"/>
       <c r="L104" s="36">
@@ -6934,8 +6934,8 @@
       <c r="I105" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J105" s="35">
-        <v>532</v>
+      <c r="J105" s="39">
+        <v>133</v>
       </c>
       <c r="K105" s="35"/>
       <c r="L105" s="36">

</xml_diff>